<commit_message>
[MPD]PL and SCH miss update
</commit_message>
<xml_diff>
--- a/2_Micro_Plasma_Dispenser/1_Schematic/Build V2.0/MPD Issue and Change list_V1.0.xlsx
+++ b/2_Micro_Plasma_Dispenser/1_Schematic/Build V2.0/MPD Issue and Change list_V1.0.xlsx
@@ -4,12 +4,12 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="14250" yWindow="765" windowWidth="14805" windowHeight="8010" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="SET" sheetId="3" r:id="rId1"/>
     <sheet name="Issue" sheetId="1" r:id="rId2"/>
-    <sheet name="MAIN" sheetId="2" r:id="rId3"/>
+    <sheet name="MAIN V2.0" sheetId="2" r:id="rId3"/>
     <sheet name="Sheet1" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="145621"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="46">
   <si>
     <t>No</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -196,6 +196,10 @@
   </si>
   <si>
     <t>LED3,4,5 역삽</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2019.11.11 Femto에 V2.0으로 release</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -205,7 +209,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
     <numFmt numFmtId="176" formatCode="&quot;#&quot;00"/>
-    <numFmt numFmtId="180" formatCode="0.0"/>
+    <numFmt numFmtId="177" formatCode="0.0"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -459,7 +463,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -555,7 +559,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="180" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="표준" xfId="0" builtinId="0"/>
@@ -991,8 +998,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B4:H21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H20" sqref="H20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G24" sqref="G24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1231,10 +1238,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:H6"/>
+  <dimension ref="B3:H7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F24" sqref="F24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1313,9 +1320,21 @@
       </c>
       <c r="H6" s="14"/>
     </row>
+    <row r="7" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B7" s="34" t="s">
+        <v>45</v>
+      </c>
+      <c r="C7" s="12"/>
+      <c r="D7" s="22"/>
+      <c r="E7" s="22"/>
+      <c r="F7" s="32"/>
+      <c r="G7" s="22"/>
+      <c r="H7" s="14"/>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Femto release Data 정리 및 MAIN PCB 수정
</commit_message>
<xml_diff>
--- a/2_Micro_Plasma_Dispenser/1_Schematic/Build V2.0/MPD Issue and Change list_V1.0.xlsx
+++ b/2_Micro_Plasma_Dispenser/1_Schematic/Build V2.0/MPD Issue and Change list_V1.0.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="14250" yWindow="765" windowWidth="14805" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="14250" yWindow="765" windowWidth="14805" windowHeight="8010" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="SET" sheetId="3" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="54">
   <si>
     <t>No</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -212,6 +212,26 @@
   </si>
   <si>
     <t>Key path에 저항 추가 : 100</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>R2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>-</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Key Noise 대책 추가</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>R18,R27</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Plasma Noise 대책</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -270,7 +290,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="14">
+  <borders count="16">
     <border>
       <left/>
       <right/>
@@ -471,11 +491,37 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -574,6 +620,12 @@
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1010,8 +1062,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B4:H21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E28" sqref="E28"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G25" sqref="G25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1256,10 +1308,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:H7"/>
+  <dimension ref="B3:H25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1349,7 +1401,198 @@
       <c r="G7" s="22"/>
       <c r="H7" s="14"/>
     </row>
+    <row r="8" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B8" s="11">
+        <v>3</v>
+      </c>
+      <c r="C8" s="35">
+        <v>43927</v>
+      </c>
+      <c r="D8" s="22">
+        <v>2</v>
+      </c>
+      <c r="E8" s="22" t="s">
+        <v>49</v>
+      </c>
+      <c r="F8" s="32" t="s">
+        <v>50</v>
+      </c>
+      <c r="G8" s="22">
+        <v>100</v>
+      </c>
+      <c r="H8" s="14" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="9" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B9" s="11">
+        <v>4</v>
+      </c>
+      <c r="C9" s="36"/>
+      <c r="D9" s="22">
+        <v>2</v>
+      </c>
+      <c r="E9" s="22" t="s">
+        <v>52</v>
+      </c>
+      <c r="F9" s="32">
+        <v>0</v>
+      </c>
+      <c r="G9" s="22">
+        <v>100</v>
+      </c>
+      <c r="H9" s="14" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="10" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B10" s="11"/>
+      <c r="C10" s="12"/>
+      <c r="D10" s="22"/>
+      <c r="E10" s="22"/>
+      <c r="F10" s="32"/>
+      <c r="G10" s="22"/>
+      <c r="H10" s="14"/>
+    </row>
+    <row r="11" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B11" s="11"/>
+      <c r="C11" s="12"/>
+      <c r="D11" s="22"/>
+      <c r="E11" s="22"/>
+      <c r="F11" s="32"/>
+      <c r="G11" s="22"/>
+      <c r="H11" s="14"/>
+    </row>
+    <row r="12" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B12" s="11"/>
+      <c r="C12" s="12"/>
+      <c r="D12" s="22"/>
+      <c r="E12" s="22"/>
+      <c r="F12" s="32"/>
+      <c r="G12" s="22"/>
+      <c r="H12" s="14"/>
+    </row>
+    <row r="13" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B13" s="11"/>
+      <c r="C13" s="12"/>
+      <c r="D13" s="22"/>
+      <c r="E13" s="22"/>
+      <c r="F13" s="32"/>
+      <c r="G13" s="22"/>
+      <c r="H13" s="14"/>
+    </row>
+    <row r="14" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B14" s="11"/>
+      <c r="C14" s="12"/>
+      <c r="D14" s="22"/>
+      <c r="E14" s="22"/>
+      <c r="F14" s="32"/>
+      <c r="G14" s="22"/>
+      <c r="H14" s="14"/>
+    </row>
+    <row r="15" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B15" s="11"/>
+      <c r="C15" s="12"/>
+      <c r="D15" s="22"/>
+      <c r="E15" s="22"/>
+      <c r="F15" s="32"/>
+      <c r="G15" s="22"/>
+      <c r="H15" s="14"/>
+    </row>
+    <row r="16" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B16" s="11"/>
+      <c r="C16" s="12"/>
+      <c r="D16" s="22"/>
+      <c r="E16" s="22"/>
+      <c r="F16" s="32"/>
+      <c r="G16" s="22"/>
+      <c r="H16" s="14"/>
+    </row>
+    <row r="17" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B17" s="11"/>
+      <c r="C17" s="12"/>
+      <c r="D17" s="22"/>
+      <c r="E17" s="22"/>
+      <c r="F17" s="32"/>
+      <c r="G17" s="22"/>
+      <c r="H17" s="14"/>
+    </row>
+    <row r="18" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B18" s="11"/>
+      <c r="C18" s="12"/>
+      <c r="D18" s="22"/>
+      <c r="E18" s="22"/>
+      <c r="F18" s="32"/>
+      <c r="G18" s="22"/>
+      <c r="H18" s="14"/>
+    </row>
+    <row r="19" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B19" s="11"/>
+      <c r="C19" s="12"/>
+      <c r="D19" s="22"/>
+      <c r="E19" s="22"/>
+      <c r="F19" s="32"/>
+      <c r="G19" s="22"/>
+      <c r="H19" s="14"/>
+    </row>
+    <row r="20" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B20" s="11"/>
+      <c r="C20" s="12"/>
+      <c r="D20" s="22"/>
+      <c r="E20" s="22"/>
+      <c r="F20" s="32"/>
+      <c r="G20" s="22"/>
+      <c r="H20" s="14"/>
+    </row>
+    <row r="21" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B21" s="11"/>
+      <c r="C21" s="12"/>
+      <c r="D21" s="22"/>
+      <c r="E21" s="22"/>
+      <c r="F21" s="32"/>
+      <c r="G21" s="22"/>
+      <c r="H21" s="14"/>
+    </row>
+    <row r="22" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B22" s="11"/>
+      <c r="C22" s="12"/>
+      <c r="D22" s="22"/>
+      <c r="E22" s="22"/>
+      <c r="F22" s="32"/>
+      <c r="G22" s="22"/>
+      <c r="H22" s="14"/>
+    </row>
+    <row r="23" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B23" s="11"/>
+      <c r="C23" s="12"/>
+      <c r="D23" s="22"/>
+      <c r="E23" s="22"/>
+      <c r="F23" s="32"/>
+      <c r="G23" s="22"/>
+      <c r="H23" s="14"/>
+    </row>
+    <row r="24" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B24" s="11"/>
+      <c r="C24" s="12"/>
+      <c r="D24" s="22"/>
+      <c r="E24" s="22"/>
+      <c r="F24" s="32"/>
+      <c r="G24" s="22"/>
+      <c r="H24" s="14"/>
+    </row>
+    <row r="25" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B25" s="11"/>
+      <c r="C25" s="12"/>
+      <c r="D25" s="22"/>
+      <c r="E25" s="22"/>
+      <c r="F25" s="32"/>
+      <c r="G25" s="22"/>
+      <c r="H25" s="14"/>
+    </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="C8:C9"/>
+  </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" r:id="rId1"/>

</xml_diff>